<commit_message>
Get daily reddit data: Tue Apr  8 08:12:37 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_13.xlsx
+++ b/data/collected_data/2025_04_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C508"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3525 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ju84lq</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Scooby- doo nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrir2k37gkte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ju83rl</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>I’m shocked at the prices people are paying in the States for their nails?! Why so expensive?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/888j8j3vfkte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ju7yng</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>beach nails</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36nyuzzwdkte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ju79zw</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>2.5 hours later…I love them!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn42xp3s4kte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ju77ey</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Black french and cute bear</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju77ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ju2fxx</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Would you pay $75 for a dip on natural nails with chrome? In Cali for reference</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju2fxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ju6fu2</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>My girlfriend and me got partner nails.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npyn7uvhujte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ju6c2k</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Wanted just french but my nail tech had a better idea 🌸</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btbf7in9tjte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ju5nxv</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Goodbye acrylics</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttdc7tugljte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ju5icr</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>green goddess 👑💚✨️</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju5icr</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ju5hna</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Possible MMA nails, removal aftercare questions?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ju5hna/possible_mma_nails_removal_aftercare_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1jtvg98</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Stilettos!</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtvg98/stilettos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1jtwgz6</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Never gotten my nails done what to expect?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u046slxmahte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ju4qwh</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Nail curves when it gets longer</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju4qwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ju54x5</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>questions about my nails in the body text, advice wanted please !</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju54x5</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ju55et</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Best nails for a month in Italy</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ju55et/best_nails_for_a_month_in_italy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ju3dgz</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Question about UV Nail Glue</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ju3dgz/question_about_uv_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ju4ib2</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Nail split into nailbed on vertical ridge, split just extends as nail grows out. Help 😭 what can I do to stop this? Tried trimming way back, didn't help.</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/g0iPtW1</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ju4xrg</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>cat eye and chrome 🦋✨</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2f75afidjte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ju4djx</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Is it obvious that the nails are too big for my nail beds?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju4djx</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ju4c50</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>My beginner GelX sets</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju4c50</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ju3z0s</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Uneven Nail Bed</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4faldal3jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ju3xrm</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>What would you name this set?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owssjhe83jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ju3v58</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Coffin is the best shape of nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fta9he0j2jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ju3ti3</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxpa6hl22jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ju3rll</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>🌸👁🌿</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13eajg1l1jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ju3rbl</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>How can I do nails think these at home</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43i9hfl01jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ju3o0h</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Spring Nails!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yfof5ql0jte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ju3cpv</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Smokey glittery shorties</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju3cpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ju3194</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Nail Artists Recommendation (Brooklyn, NY)</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ju3194/nail_artists_recommendation_brooklyn_ny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ju2pi6</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Sweet and Sour Lacquer - It's Hideous. I LOVE It!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju2pi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ju2kni</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgerznmfqite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ju2jo9</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Learning how to do gel x nails. All tips and advice are welcome!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9bxuto7qite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ju167r</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nail tech put extension under the natural nail</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju167r</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ju24kl</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Nude gel color recommendations?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emm9rxrdmite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ju209i</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>First time trying UV polish, I'm in love</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8a582383lite1</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ju1w72</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>what do you recommend?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju1w72</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ju1r8w</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Buried the stilettos and rose again in nude coffin nails. Natural? Yes. Boring? Never.</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju1r8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ju1mn2</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Ready for Easter 🐰</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xku9vv1shite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ju12li</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Decided to go with a Sakura vibe for my nails yesterday!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju12li</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ju10ga</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Nails at home for lazy people</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ju10ga/nails_at_home_for_lazy_people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ju08fh</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Maroon 😍</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2kctrl75ite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1jtzyr9</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Spring mani 🌸 I’ve been obsessed with cateye recently</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biagxawy2ite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1jtzsuk</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>just got a fill today, chose more of a spring/summery color and i’m definitely loving it :))</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtzsuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1jtzbz4</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>The assignment was “technically I’m not supposed to have nails done at work”</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyp92j0lxhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1jtw8xg</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Beetles on Press Ons?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtw8xg/beetles_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1jtz4rt</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Builder over top coat?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtz4rt/builder_over_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1jtyt9b</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Are these worth 85?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtyt9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1jtyhxv</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>I call this style "desperately seeking dopamine" 🫠</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4lmlbxipqhte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1jtyonw</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>💐 spring nails</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgaq4dcashte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1jtydvo</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>First time trying soft gel extensions</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ct8npa2tphte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1jty08x</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6anegxomhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1jtxqup</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr9jf9zjkhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1jtxm9q</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Fun lil practice painting with old Disney handwriting ☺️🫶🏼</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly129j2kjhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1jtx3uc</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Advice post my nail cracked</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5mji21lfhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1jtwj79</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Not near as fancy as the rest of y’all, but this is my first set of gel-x and I feel pretty proud of them!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rlo5w04bhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1jts47x</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Overfiled Nails - how screwed am I?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jts47x</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1jtuwt9</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Advice on these nail tips please</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo5lt4l8zgte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1jtvb1t</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Guy looking to help fiancé</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtvb1t/guy_looking_to_help_fiancé/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1jtvety</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Excuse the dryness - I was at an outdoor fair. But loo at the sparkle! 🤩</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jbece8352hte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1jtv5za</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>🌷 ILNP Spring Fairy Skittle 🌸 Thumb to pinky: Flower Child, Pixie Party, Bluebell, Pool Party, Fairy Dust ✨</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtv5za</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1jtv3n1</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Refill or start over?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtv3n1</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1jtuvim</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Press on Nail Sizes to MM?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtuvim/press_on_nail_sizes_to_mm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1jtuqpw</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>I’ve been obsessed with 3D flowers lately.</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtuqpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1jtukln</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>been into wearing builder gel by itself recently. clear structured nails look so dang good!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtukln</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1jtuh2b</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Cute💍</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/forestgreenuntidyamericanredsquirrel</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1jtu9x3</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Pointy almond or coffin?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtu9x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1jtu37k</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Your favorite polish remover</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtu37k/your_favorite_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1jttg7b</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Classes for character nails??</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfjis0fqogte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1jtt4er</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>What goes well with this dress?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtt4er</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1jtsgkc</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>My friend did my nails!!</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtsgkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1jts07s</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>I love my new chrome tribal spring nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jts07s</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1jtrlku</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Jungle Book Press Ons - by Nikki Nailed it 💜</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o52ywrsgbgte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1jtrc00</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My Take On Glass Nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtrc00</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1jtqtnx</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>nailart ideas for geto suguru from jujutsu kaisen, please..?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtqtnx/nailart_ideas_for_geto_suguru_from_jujutsu_kaisen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1jtqwbn</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Acrylic/gel/biab/sns?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtqwbn/acrylicgelbiabsns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1jtqoxv</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Easter</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pecbigw4gte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1jtqj23</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>2000s neon grunge</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqczfjoq3gte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1jtq1la</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Lots of shine ✨ ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agpqh2n90gte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1jtpx9n</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>I did my best friend and I’s nails, which do you like better?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpwty6iezfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1jtpoxf</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>My nicest DIY set so far</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kzi99fdzwfte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1jtpdzk</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>I started working with gel a couple of months ago but have years of using regular polish and stamping plates. Some of the stuff I've done so far</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qmwydtgvfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1jtpdl3</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Which nail shape looks best on my natural nails? Pointed or Oval?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtpdl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1jtoxmb</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>clown nails 🤡</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/acih7ui2sfte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1jtnxnz</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Nail with heena, why not?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtnxnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1jtnrll</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Bees</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtnrll</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1jtnqf9</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>My nailtech did a good job</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtnqf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1jte7gs</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>ring of fire?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18vbmbr1qcte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1jtdvx9</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Heeeeellllppppp</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25lj8sx2mcte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1jti9ee</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Jhope Concert nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ni8txgr6ete1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1jtjsrh</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>damaged nail bed?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtjsrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1jtkkwf</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Press On Nails - Hypoallergenic Nail Glue Available Anywhere?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtkkwf/press_on_nails_hypoallergenic_nail_glue_available/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1jtl9f7</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>How do I avoid my BIAB from horizontal cracking?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzirg1o80fte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1jtldso</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Tried a new nail tech even though I love my old one</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtldso</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1jtmvlv</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Spring color! What do u think?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtmvlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1jtmkfh</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I can not stop staring at this set I did</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9w8srvnafte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1jtmg5f</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>First Time Getting Builder Gel. I love it!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtmg5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1jtldzx</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Purple marble, pearl, &amp; gold set</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtldzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1jtl8h7</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7e7exf00fte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1jtl87r</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Is builder gel necessary?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jtl87r/is_builder_gel_necessary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ju83zt</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Off the Deep End</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju83zt</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1jty3r0</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Fastest Drying Indie Polish?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jty3r0/fastest_drying_indie_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ju3356</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Oldie but goodie</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/03lk2gq4vite1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ju7vmw</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Revlon nail polish moldy?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju7vmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ju7mo5</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Speckle cuteness</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju7mo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ju7841</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Creme and jelly duo for extra shine ✨️</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju7841</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ju76c5</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Celebrating 4 months of no biting with a lavender skittle</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dq0wm4g3kte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ju6w96</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Can anyone ID this color?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ju6w96/can_anyone_id_this_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ju639w</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>matching with my phone case ⭐️</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0up806dqjte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ju4udq</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Acrylic Nails with Contact Dermatitis</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ju4udq/acrylic_nails_with_contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ju4k3h</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>BKL Fake Dating</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju4k3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ju43q5</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>How do I get my hands on the new BKL magnetics?!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ju43q5/how_do_i_get_my_hands_on_the_new_bkl_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ju36gq</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Magenta for days</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/houapfgyvite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ju34mg</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Celebrating almost 1 year of no nail-biting!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ju34mg/celebrating_almost_1_year_of_no_nailbiting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ju2tfx</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>ISO polishes that look like mold/bacteria</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ju2tfx/iso_polishes_that_look_like_moldbacteria/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ju2p01</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Sweet and Sour Lacquer - It's Hideous. I LOVE It!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju2p01</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ju20ls</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Extra Credit</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky9t21kclite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ju1w2j</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Painted Polish- Broccoli Biology: shiny and matte</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju1w2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ju1i1j</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Who says you can’t wear vampy in spring ;)</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1eiehamgite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ju17ph</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>But Do Aliens Believe in Me?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju17ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ju0jt6</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>$1.50?!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju0jt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ju049o</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>ILNP Ava💜🧡</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju049o</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ju03ra</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer mishap or just how the polish is?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/402terh44ite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1jtzy7r</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>ILNP whisper and amber</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfhhqffu2ite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1jtzils</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Thank you to whoever posted Enchantmint the other day!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nohgi0v2zhte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1jtzhf2</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer - Dragon Darts</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lpqclzsixhte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1jtz22v</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>KBShimmer Love 🪨💎</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtz22v</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1jtyv8i</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>“We have Enchanted Mist at home”</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtyv8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1jtyltq</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Same, girl. Same.</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtyltq</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1jty93y</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Hi girlies! Looking for an Essie or Opi colour like this? Isn’t toooo purply and isn’t tooo blue either. Help! 🤪</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwmexeepohte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1jtxua1</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>I call this "desperately seeking dopamine" 🫠 (very necessary for me while trying to stay sane in the US right now)</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lhrf2c2blhte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1jtxdks</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Cracks?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cvo9l0phhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1jtwkfy</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>happy colors! 🩵💚🩷</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtwkfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1jtwern</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Bright purple with pink flakes</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qoe29ln6ahte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1jtwcrv</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Happy Haunts</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtwcrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1jto1p4</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Are my press-ons horrible? How can I improve?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jto1p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1jtt61n</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Someone else feels that getting their nails done gives them a boost, it always makes me feel good 🤗</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk23nszrmgte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1jttjnf</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>long shot - color dupes for Lights Lacquer Cubana?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jttjnf/long_shot_color_dupes_for_lights_lacquer_cubana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1jtvnpx</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Shifty galore!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/juq7j9co4hte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1jtvlrs</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Is there a polish like this one?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7hrr1za4hte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1jtvcnt</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Playing with purples</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtvcnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1jtv2qw</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>🌷 ILNP Spring Fairy Skittle 🌸 Thumb to pinky: Flower Child, Pixie Party, Bluebell, Pool Party, Fairy Dust ✨</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtv2qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1jtunhd</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>First time buying a “fancy” polish after years of biting!! Mooncat “imperial storm trooper”</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtunhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1jtugd6</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Acrylate Allergy from Nail Glue?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jtugd6/acrylate_allergy_from_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1jtu39v</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Orly Bonder base coat WRECKED my nails.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jtu39v/orly_bonder_base_coat_wrecked_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1jtthst</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Mooncat Sand Viper</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtthst</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1jtt710</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>For the love of reflectives💖</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vo276urwmgte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1jtt4y7</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Match made in heaven</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mn102mdjmgte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1jtt2sx</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>What nail shape suits me best</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtt2sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1jtt11g</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Update: I got the job! ✨🎉🎊🎇🎆✨</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ato9rtcrlgte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1jtsyoz</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Wow!! You ladies weren’t kidding about BKL!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krda7dkalgte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1jtsk1c</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>My new fav!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtsk1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1jtsg41</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Accidentally coordinating with Neck Oil 💀</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtsg41</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1jtscl7</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Black jelly is fulfilling my inner emo and clean girl at the same time</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtscl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1jtsa9c</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>strawberries for spring 🍓</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtsa9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1jts6pv</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>rain &amp; daffodil season 🌼</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jts6pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1jts4q4</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>What do swatchers do with all of the polishes they receive?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jts4q4/what_do_swatchers_do_with_all_of_the_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1jts21i</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>It’s spring time but I’m angry</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jts21i</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1jtrvha</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>First time using magnetics 😍</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j9538sgbdgte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1jtrs1e</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>One good thing about short nail beds</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtrs1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1jtr7k4</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>ISO non-gel polish like this old one</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtr7k4</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1jtr68v</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Blurring Basecoat/sheer jelly?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jtr68v/blurring_basecoatsheer_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1jtqtkr</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>This blue 😍</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtqtkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1jtqjwf</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Starrily Northern Lights collection</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhnc1qjw3gte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1jtqgpv</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>WARNING! Broken nail pic. Silk wrap repair advice needed.</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtqgpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1jtq64m</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Can't stop staring at this greeeeen</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y39ol2a61gte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1jtp1ht</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Spring Skittle</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtp1ht</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1jtotgd</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Love this little gift with polish</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hopenvxbrfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1jtotdz</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Can I get opinions?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsrpkqkbrfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1jtopyx</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Cracked appreciation post 🩷💜✨</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h39gu9v9pfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1jtokek</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>holo taco “touch grass” dupe?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5w8lwhipfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1jtoj50</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>thoughts on dazzle dry + using dazzle dry with regular polish</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc2ydjzemfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1jto0i8</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Do any of you have polishes you’ve avoided just because you hate the name?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nez9mecdlfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1jtny42</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Whimsical pink L.A. Colors topper 💕🧚🏾</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtny42</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1jtnx25</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>love this hot pink</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtptj24okfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1jtmw9k</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Not impatient for my first Emily de Molly delivery, nope nope nope</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qiqm9my5dfte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1jtm8qt</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Chilly spring corporate Monday Mani</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtm8qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1jtlze3</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Experiments in sponging on disappointing Mooncat polishes</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtlze3</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1jtlvrl</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Colored Pencils in Nail Polish!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtlvrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1jtlnbc</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>At a certain angle your holo rainbow becomes round!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbxj1j173fte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1jtlbbh</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I asked ChatGPT on what nail design I should do next!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtlbbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1jtkx7h</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Made a jelly out of a clear polish and some red, I am obsessed with this colour and would love any recs for polishes that are similar!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtkx7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1jtkwmg</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Atomic Rum Ham + Lurid Conviction = metallic Narf</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtkwmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1jtkii1</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Goal: BRIGHT, Mission: ACCOMPLISHED</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fagsk2eptete1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1jtk9gm</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Dark matter velvetized</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/10cn2zxpqete1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1jtjpr9</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Been on a red hunt and everyone I try I fall more in love with 🥰🍒♥️🌶️</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtjpr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1jthn9a</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jthn9a/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1jt5ysy</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>So GLOWY ✨️</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jt5ysy</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1jt8i99</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>HELP! My nails are so stained</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikpxrkja3bte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1jt94yt</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Ready for spring</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ryafcvu79bte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1jtgfvm</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>My Job is Beach, had to make do with a lake instead though.</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtgfvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ju70bc</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Spring Nail Art</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju70bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ju13nz</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>my second set!!!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqart6d0dite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ju09rb</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>My favorite</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90oubeti5ite1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1jtzl7q</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Gel Nails I Did Yesterday</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtzl7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1jtxmr7</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Practising some Disney font 🥰</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u45y89gnjhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1jtxfvx</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Spring Fever</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbrtlbi4ihte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1jtwsws</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Done by Maria at Apple pink nails 💅</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spaodo46dhte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1jtvngj</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Shark Nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtvngj</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1jturt4</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Not sure I like it</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jturt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1jtujcz</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>I’ve been obsessed with 3D flowers lately.</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtujcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1jtrd4e</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>My take on glass nails 🪞💎</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtrd4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1jto7nv</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Press on advice! See info ⬇️</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jto7nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1jtnvhw</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>My very first set for a customer!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtnvhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1jtlq3b</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>My Nail Charm Bar 💅</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t3ak24p34fte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1jtlg0k</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Purple marble, pearl, &amp; gold set</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jtlg0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1jtju8p</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Trying to get better at gel nail art!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4teorainete1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr  9 08:12:09 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_13.xlsx
+++ b/data/collected_data/2025_04_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C508"/>
+  <dimension ref="A1:C693"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9069,6 +9069,3151 @@
         </is>
       </c>
     </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1jv04qy</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>My natural nails keep breaking</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jv04qy/my_natural_nails_keep_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1juzy75</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>strawberry nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kozyjzagrte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1juzwlm</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>love how it turns out!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlk7nebpfrte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1juztb1</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Proud!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juztb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1juzqwf</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>searching for a shade like essie chocolate cakes</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juzqwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1juyrbg</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I was a model for a friend who is starting in the nail world, I loved her design😍</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rj9whru0rte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1juynm9</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>What do you think of my new nails? 🤭</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x4foklnzqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1juy8p7</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Bright but subtle (for me)</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juy8p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1juy5hu</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>This month's nails😍</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4eopo3otqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1juxvs1</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>This was my first time getting little jewels added. It turned out so cute!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bpnz21kqqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1juxtwp</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>feels weird to say these are my natural nails when theyre covered in gel, so i will instead say natural length! no extensions!!!!!!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p55lys2ypqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1juxlh5</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>My april nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pq2vjgcnqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1juxcch</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Baby boomer technique, I like the natural</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b33whmekkqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1juxa94</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>What is the best nail oil for natural growth?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juxa94/what_is_the_best_nail_oil_for_natural_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1jux7ie</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>soft &amp; basic</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddqg7n15jqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1juwxv7</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>first time getting builder gel!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juwxv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1juvbv9</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Need help!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juvbv9/need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1juuqa0</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Onycholysis questions</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juuqa0/onycholysis_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1juwjeq</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Long nails and contacts</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juwjeq/long_nails_and_contacts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1juvits</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>How bad are these nails? Should I go back?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juvits</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1juw9ax</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Best nail options?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juw9ax/best_nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1juvfg8</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Real question.</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tk3eygc1qte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1juv6nc</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Love this 💖 chrome 💞</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxjavskzypte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1juv28g</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best? Thanks everyone 🌼</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juv28g</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1juumk9</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>New Nail set</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z25zdbyvtpte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1juug14</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Loving my newest Spring nails!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juug14</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1jutwrb</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Possible silly question about options!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/719u8ub9npte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1jutmx0</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Spring nails! 🌺 🦋</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jutmx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1juthyy</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Got my first acrylic set today…</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juthyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1jut5fi</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Nails🌸🌸</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6ng0cyagpte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1jut3xb</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Cherry blossom and koi nails 🌸</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jut3xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1jut1of</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Gel dupes/similar to Mooncat?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jut1of</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1jut08m</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Red Nail swatch</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jut08m</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1jusqpm</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>I have no idea what to do</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jusqpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1jusm2d</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Yep, they’re mine!</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jusm2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1jus4yk</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in a very long time. I love them and can't wait to keep doing them</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jus4yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1jurqvi</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Concert Nails! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jurqvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1jurg8f</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Spring is here 🌷</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jurg8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1jup0j9</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Is this normal for a nail tech to do?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jup0j9/is_this_normal_for_a_nail_tech_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1jur8mu</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Mood nails, courtesy of my husband! 💙</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jur8mu</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1jur7i5</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Tip of nail broke</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79kzoigdzote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1jur6sr</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>They’re not even the same shape!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4i9ebrq7zote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1jur5xj</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Has anyone ever broken out in a rash after using DIY gel nail kits?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jur5xj/has_anyone_ever_broken_out_in_a_rash_after_using/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1juqycq</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>What am I doing wrong</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juqycq</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1juqx1r</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Doing my nails myself</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juqx1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1juqlvh</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Diy blueberry set</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psldiwtcuote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1juq8sj</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Easter egg press-ons i made last night 🐣</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juq8sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1juq56m</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Give honest advice</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juq56m</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1juq2me</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Gel lifting</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84rp1quzpote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1juoyyn</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Nail Hack</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n31242chhote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1juoxu3</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Decided I’d go Shorter</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juoxu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1juovo7</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juovo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1juoih9</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Need advice!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juoih9</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1juoioq</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>little sister did my nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gb1mwf3eote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1juoibf</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>dancing soot sprite nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juoibf</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1juofoz</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>To remove or not remove</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whm9dwdhdote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1junz63</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Set for cuba</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0j6p5q0aote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1junywp</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Distracted by my own nails at work</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knzht31y9ote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1junujy</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>What do you think :) Beginner here</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1junujy</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1juns7a</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Good strengthening polish?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juns7a/good_strengthening_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1junnx1</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Am I overreacting? Is this normal?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1junnx1/am_i_overreacting_is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1junly4</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>So glad I went with the brighter pink</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1junly4</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1junjzt</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>My friend got her nail license  and did my nails!! Spring edition! 🐛🐞</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1junjzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1julvoq</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>New nail tech and not sure, would like some opinions</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1julvoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1jum4h4</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>How to isolate nail tip?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jum4h4/how_to_isolate_nail_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1jumy6d</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Fingers ALWAYS cut up since moving back to US</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd4mcsyf2ote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1jumkcj</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Current nail paint</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jumkcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1jumfox</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Gelx on my friend 🏁🎱⭐️</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9li1lomynte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1julcou</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Nail shaping tips?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ut97hzjqnte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1julal8</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>kapping dark brown</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tofrbcz2qnte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1juktnz</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Glamnetic remover</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juktnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1jukt7v</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Slowly getting better… I have an audition on Friday for a musical set in the 1930’s wanted something of that “vibe”</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jukt7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1jukhe8</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Orchid Nails</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frehbp6aknte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1jukgc6</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Went to a soft pink jelly for warm weather vibes 🌸</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jukgc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1jukfuc</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Decided to do something a little basic compared to what I normally get. Simple but classy for this set 💅</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tlniefzjnte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1juk5qb</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Mooncat Fleur Sauvage</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rfvu7vuhnte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1jujt5q</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Where can I find clippers smaller than 2”?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jujt5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1juj199</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Girly but simple, I love them</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwzrjdi3ante1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1juihhg</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Just want to show my nails here, first time post!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzwuybr46nte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1juhh81</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Beginner question, what do I do with my gel nails that are growing out and lifting in the back?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1juhh81/beginner_question_what_do_i_do_with_my_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1jugxys</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>If I gave myself an allergic reaction to GelX/gel, should I try dip?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jugxys/if_i_gave_myself_an_allergic_reaction_to_gelxgel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1juhmol</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>New salon opened near me, took the risk 😍</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oshrgdtszmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1juhgcz</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>obsessed with lilac</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l6xknxriymte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1juh0jf</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>pr for length! time to say goodbye 🫡</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe37s00cvmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1jugw15</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Just started doing my own builder gel myself. Is it too bulky or are my nails just weird?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jugw15</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1jugufo</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Moo</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jugufo</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1jugu1u</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>First time getting Gel-X and I’m in love</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yatp0bztmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1jugoil</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>🐮</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jugoil</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1jug6e7</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>FILL?!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fzgbww3pmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1jufok3</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Strawberry Nails</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jufok3</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1juf9u6</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juf9u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1juf2dp</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I offer the council….</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1htxsmjugmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1jueqw4</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>First time doing nail art</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a1djppfemte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1jueko1</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>It’s giving fruit of the loom</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jueko1</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1judizc</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>pointy almond, rounded almond, or coffin? which looks better?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1judizc</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1juehox</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>What nail shape would look good on me and what design?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9bxftofcmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1juegl8</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I’m obsessed with these!!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txeyxbv6cmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ju76rh</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Some designs I've had over the years!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ju76rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1ju73wz</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>OMG these nails represent me I love them😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vj6rrrl2kte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1jue5lz</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>I'm always indecisive about my nail color, but red is always a good choice. Fall is here.</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyzkznrt9mte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1juy7dn</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>I need a nail polish in every single one of these tiles 😩</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he0g8a39uqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1juwxv1</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Favorite polish recommendation</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1juwxv1/favorite_polish_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1juwjpa</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>check out this adorable pink jelly from la colors</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juwjpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1juwiku</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Atomic polish</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1juwiku/atomic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1juvp6a</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer - Spicy</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l64r4zxw3qte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1juudth</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>China Glaze - Rainbow 🤍</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juudth</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1juu8i9</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Mooncat Smoothing Base vs. KBShimmers</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1juu8i9/mooncat_smoothing_base_vs_kbshimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1juu4ry</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>stank-free storage for kbshimmer polish thinner?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1juu4ry/stankfree_storage_for_kbshimmer_polish_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1jusp2c</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Bikini so teeny dip powder?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jusp2c/bikini_so_teeny_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1jusnlw</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Looking for white/ ivory/ bridal polish that is flattering for tan skin</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u5q82bubpte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1jusngt</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Topcoat Request Post #1,538 (Probably). Non-toluene</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jusngt/topcoat_request_post_1538_probably_nontoluene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1juslus</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>This is your sign to match your nails to your Crocs 💕 (or vice versa)</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juslus</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1juslr0</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Lurid Unyielding and NOL Prepared for any &amp; all Scenarios</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juslr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1jus9gg</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Where did this pose come from?  I think it makes human hands look like chicken hands with a tiny wrist... Am I crazy?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o742a6ps6pte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1jus575</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>first time attempting mismatched nails and I’m not sure how I feel about it</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y84qw76b7pte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1jus096</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>The many faces of a thermal</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jus096</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1juru56</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>New polish!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/krcy2pmm4pte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1jurttt</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Black Honey Nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mue909bk4pte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1jurjsi</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Me holding the bottle of Ether Dragon I just got, wearing Checkmate</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jurjsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1jured4</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>I love patchwork nails so much 🥹</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jured4</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1jupppt</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Storm inspired</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jupppt</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1jupib2</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Glazed donut 🍩</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jupib2</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1jup9qm</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Springtime nails! Same color as my budding redbud tree</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jup9qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1jup5fe</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Halfway through the battle bracket!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jup5fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1juoxyn</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Dupe for Sally Hansen Triple Strong</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1juoxyn/dupe_for_sally_hansen_triple_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1juoooi</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer: Dance of the Sugar Plum Fairy</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx9wwc9cfote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1junvwk</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Gahh duped myself</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1junvwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1junpau</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Finally swatched my collection!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1junpau</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1juni0p</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>This week's nails were inspired by trash</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1di2ezug6ote1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1jumkye</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>When your nails accidentally match your popsocket.</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tj85kqpznte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1jumjy2</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Yucca in Bloom: a photochromatic with baggage</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jumjy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1jume6k</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Sad swatcher news</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pu1cl0bynte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1julh69</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Enchantmint + Sparrow 😍</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6q51yk1hrnte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1juledh</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>BKL's "Or from beyond?" is absolutely stunning</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juledh</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1jukorv</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>This will be my pose until my index nail grows out</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jukorv</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1juek0h</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>I’m Beautiful. I’m Mad. I Can’t Stop Staring.</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juek0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1jukg3o</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>What if I told you this polish was €1.29?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jukg3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1juhetv</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Prugly and proud!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juhetv</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1jujych</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>The objectively stunning “A Comet’s Tale”</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dkhgebkmgnte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1jujhk3</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Run, do not walk and purchase this stunner pronto</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jujhk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1jujh06</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Cheap drugstore peel off basecoat?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jujh06/cheap_drugstore_peel_off_basecoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1juj69p</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>How strong are the SJ3 Designs velvet magnet?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1juj69p/how_strong_are_the_sj3_designs_velvet_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1juii6t</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Catfished over black is gorgeous!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juii6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1juigf7</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Coronation + Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juigf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1juhs8h</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Velvet Troubleshooting</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juhs8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1juho5x</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Matchy Matchy</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vibwcl30nte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1juhldg</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Speckled goth egg</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juhldg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1juh4kj</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>✨️🌈Shimmery Gradient🌈✨️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juh4kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1jugywq</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Did you need to get use to wearing polish? Do you like certain colors more when your nails are a different length?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jugywq/did_you_need_to_get_use_to_wearing_polish_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1jugtmw</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Something something smoke on the water</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr1aj5nwtmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1jugnmo</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Growing collection - Helmer</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1wj44mnsmte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1jug5f6</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Matching my nails to my hair and outfit</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jug5f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1jug0vk</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>True pearl/frosted finish polishes</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jug0vk/true_pearlfrosted_finish_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1jufwq0</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Can you magnetize nail polish with just a regular magnet wand?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jufwq0/can_you_magnetize_nail_polish_with_just_a_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1jufuhs</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Sheer Nails that are Beginner Friendly (Tips &amp; Recs)</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jufuhs/sheer_nails_that_are_beginner_friendly_tips_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1juern5</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Cracked is retiring 45 shades</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juern5</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1judv96</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Ready for dandelion season</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1judv96</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1judqf2</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>I had the craziest dream about my nails last night.</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1judqf2/i_had_the_craziest_dream_about_my_nails_last_night/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1judbuz</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Anyone know what Essie color or other drugstore brand would give me this pink?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytbwkhz03mte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1jud907</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>I still have no words.</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/35xg9hi72mte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1jud23g</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>I did (mostly) green manis for March</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jud23g</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1jubsxg</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>How Does One…?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jubsxg/how_does_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1jubrn4</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>What I wore in March</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jubrn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1jubqf6</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>jelly matchy!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fkomffkolte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1jubkvn</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Stiletto nails!💅</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrcx1kp2nlte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1juaknn</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>my attempt at cherry blossom nails 🌸</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7imuo1y6clte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1jua6zc</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Emily de Molly - The same dream</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jua6zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1juxlpb</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Howl’s moving castle 🩵</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8e95kafnqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1juxk9p</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Does anyone know which brand and colour 🥹</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juxk9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1juw7qx</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Diamondback red nail polish color?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1juw7qx/diamondback_red_nail_polish_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1juvzln</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Simple blue with lines design</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiqkvpnq6qte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1juufgv</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Anime eye mood board set</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utr22fw1spte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1juub7t</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>holographic frenchies!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juub7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1jutth9</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Obsessed with these 🪐✨</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxzthvnfmpte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1jut4ct</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>April Cherry Blossoms 🌸🌸</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8cssxg0gpte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1juq714</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Easter egg press-ons I made last night🐣</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juq714</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1junq49</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>April 💕🔵🟠💕</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1junq49</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1juk4ty</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Wanted to try Beach Vibe nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/him39y8thnte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1juih42</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Spring Watercolors</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykzb3t626nte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1jugv6g</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Moo</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jugv6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1jugelx</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>New Set!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7310vcsqmte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1jugdrq</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Wiping gel nails with acetone</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jugdrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1judnmi</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Death Grips nail art as the boys are BACK 🖤</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwqteimp5mte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1jubb15</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Happy Easter 🐰 🐥</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jubb15</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1jth91n</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Hand-painted ELLIE (BELLA RAMSEY) from The Last of Us</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jth91n</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr 10 08:12:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_13.xlsx
+++ b/data/collected_data/2025_04_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C693"/>
+  <dimension ref="A1:C876"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12214,6 +12214,3117 @@
         </is>
       </c>
     </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1jvs5qg</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Any ridge filler polish for deeply ridged/indented nails? UK</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1w7c5vhmyte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1jvsa3b</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Boyf paid for my nails</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ya7k5u3oyte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1jvs69s</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Went for a cute spring vibe do you like?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nobz3j1pmyte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1jvs1cj</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Pink jelly gel nails, what do we think?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvs1cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1jvrgej</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>a touch of love to my beautiful nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybjstk5ddyte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1jvr9rl</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Rate my nails..</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvr9rl/rate_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1jvprs2</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I have been biting my nails for more than 17 years and I'm 20, I wanna use press on nails to stop, will it work on these nails?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwtwxfr7txte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1jvr1ie</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cn00s21a8yte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1jvqic7</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>HELP! My favorite coffin nails are no longer available.  Would anyone know where I could find these or similar?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlbrixt30yte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1jvph75</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Does this acrylic mistake increase risk of infection?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvph75</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1jvp7fa</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My nails… the way to my nailtech’s studio</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvp7fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1jvou5w</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Love my nail tech</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvou5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1jvni6f</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Had to cut two of my acrylic nails. What do I ask for to get them redone?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvni6f/had_to_cut_two_of_my_acrylic_nails_what_do_i_ask/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1jvno1q</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Nails chosen for a night out</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p01hinw97xte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1jvnk2s</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>little ladybugs 🐞</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvnk2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1jvndba</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Is there uv gloves for toes?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvndba/is_there_uv_gloves_for_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1jvn52s</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Birthday Nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t16p2ipb2xte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1jvn4hz</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Loving the pink for spring! 🌸</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsbrza162xte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1jvn1mf</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>First Time Nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i51iqmje1xte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1jvn03c</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>♥️</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q53px3701xte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1jvmz24</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>How are the cuticles looking?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v41xc8q0xte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1jvmubn</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Glow in the dark easter nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmubn</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1jvmjbu</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Chocolate Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmjbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1jvmo7k</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Spring Set</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmo7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1jvmo68</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>How I love being a woman 💛🌟🐝🐥🍋🍯🔆✨💫</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmo68</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1jvme0s</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Gel Nail Help</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvme0s/gel_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1jvmaoh</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Which nail shape is your favorite?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4sggynduwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1jvm1vl</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>I don’t know how to feel about my nails</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvm1vl</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1jvm5qu</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Is it rude to say your experience was mixed when asked how your experience was?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvm5qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1jvm5t8</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Decided to try cat eye for the first time!</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8xokx83twte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1jvlzlp</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Not a nail pic but discussing prom nails!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvlzlp/not_a_nail_pic_but_discussing_prom_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1jvlz2y</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Extremely weak nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvlz2y/extremely_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1jvlq9z</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Tried my best to capture the gorgeousness and depth I’m obsessed with this magnetic!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvlq9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1jvlch2</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Spring in Paris or Something Like That (spring/summer inspo welcome!)</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvlch2</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1jvlf6k</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Nut Based Products</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvlf6k/nut_based_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1jvlkf5</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Leaf Bug Nails!!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvlkf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1jvlj62</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>🧿🖤</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdyzaiw9nwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1jvleb1</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Got my first french manicure!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvleb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1jvl4zm</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>I stopped biting my nails 3 years ago</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv0zf76mjwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1jvk86d</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Broken nail help.</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb5itgobbwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1jvl0i1</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Where to buy supplies?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvl0i1/where_to_buy_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1jvkur8</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Taking gel polish through airport security</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvkur8/taking_gel_polish_through_airport_security/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1jvkew7</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>yin &amp; yang hearts 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uylwiusvcwte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1jvk9tk</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Back to short nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgozhd1rbwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1jvjmg7</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Gap?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqa7mir26wte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1jvjj0f</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Hand painted (watercolor art)</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk27b6e85wte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1jvjcqu</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvf6e8bs3wte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1jvi93y</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>French tip stickers</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34lqu6usuvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1jvhcgk</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2go415ennvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1jvip6x</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>I forgot to post my last set so here’s the latest 2!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvip6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1jvidfd</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>French with cute flowers</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3293q6rvvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1jvia6r</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>blue chrome !!!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m85nq3i0vvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1jvhx1u</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Flowers for spring!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvhx1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1jvhsrv</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Diamonds and pink!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvhsrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1jvhsjl</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Looking for nail color suggestions !!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvhsjl/looking_for_nail_color_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1jvhs3u</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>I did my nails instead of studying :)</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvhs3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1jvhaqq</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Natural nail broke</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvhaqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1jvhio8</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>I'm trying to grow out my nails so I did a new polish</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jif1c6qzovte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1jvgd5g</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>In my Victorian era</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u77m5k7gvte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1jvh24i</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Been a long long time since I’ve done my own nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my9oo8chlvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1jvgn1h</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>just so happy</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgn1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1jvgi5c</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>What shape would fit my nails the best?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgi5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1jvghmh</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>MRI and cat eye polish</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvghmh/mri_and_cat_eye_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1jvfoj5</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>What colours are we thinking for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go3l6o5yavte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1jvfd2a</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Just got my nails done for the first time! They arent really what I wanted at first, but I still like em</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvfd2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1jvf9rm</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>lifting</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvf9rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1jvfijo</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Summer ☀️ 💅</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n39r87mt9vte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1jvf9j2</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Does anyone else find doing their own nails relaxing? I did this set post seasonal depression✋🏻🙂‍↕️💅🏻</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvf9j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1jvf1q3</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Love doing ombre lately!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9evgwh6f6vte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1jvdqa4</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>What is this dip in my nail?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvdqa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1jve3id</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Irregular nail</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcpsp5lbzute1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1jves7d</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>How much would you pay for these nails? Dip, chrome, tips for length, and cuticle trim</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16v4h9cg4vte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1jvev9i</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Trying something new!</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwac7xg25vte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1jveajz</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Curved in nails?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jveajz</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1jve0tt</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Just did my nails 🥰😍</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x6zzn8syute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1jvdv9n</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Love my nails</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7isb0rnnxute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1jvdrja</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>What's the best type of manicure for your nails?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvdrja/whats_the_best_type_of_manicure_for_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1jvdp34</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Fresh polish</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv1eufngwute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1jvd78f</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Do not really like em</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvd78f</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1jvb0i2</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>My new obsession,am i good at posing?? And which one is better??</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvb0i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1jvcw3z</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>It's the brightness and boldness of the colour that makes me swoon</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buj9kx3lqute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1jvct4h</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Q for the Press-on nail girlies</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvct4h/q_for_the_presson_nail_girlies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1jvcs6q</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Nail Design</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sao5z6kspute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1jvcdou</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Cat eyes in lowlight ✨</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3rd8wy4wmute1</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1jvca9v</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>About 2 weeks of growth!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpvz997amute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1jv1f64</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>My first glow in the dark nails!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv1f64</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1juzhmn</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>I feel like these are my first successful ones</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1juzhmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1juyis2</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>is there any coming back from this?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/818iacm0yqte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1jv6b3c</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>I wore my nail inspo!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv6b3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1jv7bmz</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Are these too thick, or am I just overthinking it?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv7bmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1jv9ws0</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Splitting and weak nails</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jv9ws0/splitting_and_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1jvaizn</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Wedding SOS! Clueless bride walks into a salon…and gets burned :(</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otop3qom9ute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1jvawez</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Why does my polish have these waves?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cff7hmbcute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1jvblqo</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>How would you improve these?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvblqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1jvbmy1</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>What shape looks better</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvbmy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1jvb4qy</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Finally got cat eyes 😸</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ujclrs80eute1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1jvaztn</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Anyone know of any press ons that match this color? Need some nails for prom.</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lk90f8jycute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1jvazoy</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Nails I got done last Sunday!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umwrc4evcute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1jvaolx</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Recommendations please</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvaolx/recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1jvaj5b</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Best Nail Growth Oil</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvaj5b/best_nail_growth_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1jvrh6k</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>In love ♡</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hvqj2x6dyte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1jvqo43</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Normal polish convert 🙆🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ib093fs3yte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1jvqhdu</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Matching Nail/Lip Combos</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifbyn8nj1yte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1jvoqt2</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Anyone have a good US mail forwarding service recommendation?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvoqt2/anyone_have_a_good_us_mail_forwarding_service/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1jvnznf</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Gorgeous combo</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvnznf</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1jvnlwd</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Gorgeous deep blue dollar store jelly!</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajk9qj1p6xte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1jvnjrz</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>New favorite polish</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvnjrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1jvnf43</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>How Noble!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvnf43</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1jvmrwo</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>First time velvetizing 💜 🔮</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmrwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1jvmexj</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Twilight Sonata</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmexj</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1jvm4uc</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Treachery In The Blue</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvm4uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1jvm4g6</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>My mistake. (Inspired by someone else's post the other day)</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvm4g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1jvm0z0</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Celebrating warmer weather 🍒</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvm0z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1jvkyc3</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Dupe Request! DND Voodoo</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/198pht0whwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1jvkwco</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Mooncat Sheep's Clothing</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvkwco</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1jvkfex</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Everything Is Lit</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvkfex</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1jvk3m2</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Welp.</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fev9clj7awte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1jvjxh7</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Love 💙</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvjxh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1jvjb9m</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Best emerald green polish?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvjb9m/best_emerald_green_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1jvir18</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Pastel skittle 🌼🌷</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spp6tqxsyvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1jvimw3</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I have a thermal problem</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvimw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1jvieas</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>swatch party 🎉</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g95d8vqxvvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1jvi007</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Best white you have ever used?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvi007/best_white_you_have_ever_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1jvhy9u</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>First Clionadh mani and you were all right 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/12h7jo7esvte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1jvh6jx</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Treating/preventing keratin granulations</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvh6jx/treatingpreventing_keratin_granulations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1jvh0k0</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Can anyone guide me on how to ship polish to Australia from the US?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvh0k0/can_anyone_guide_me_on_how_to_ship_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1jvgu0k</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Sea-ing is believing</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgu0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1jvgt76</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Cute story</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w3axbjmjvte1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1jvgobs</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>My dream polish was a disappointment, so I made it myself!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1jvgo49</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Devastation &amp; Rebirth</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgo49</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1jvgk8d</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Obsessed 🌞</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgk8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1jvfeaa</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>New BKL fan has a question!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvfeaa/new_bkl_fan_has_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1jvfajh</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>lifting</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvfajh</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1jvf3rd</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>I’m so impressed with the beating this has taken.</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvf3rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1jve2u1</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Color Club Mostly Mystery Haul</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5szrbyp6zute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1jvdwzi</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>I got a 2nd The Bubbles *Free* from HHC without ordering it... This happen to anybody else?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvdwzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1jvddxl</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Abe Gets Possessive</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvddxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1jvd3u9</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>I was going to be done with magnetics, then I found holo magnetics</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iwaisuq3sute1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1jvcrg5</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Betty Draper Dupe (of color - subtle finishes ok!)</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqhxditdpute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1jvcnkv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Really struggled to get pics that do it justice, and I feel like I wasted it with my nails so short right now, but I’m so in love with ILNP Interstellar</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvcnkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1jvcer5</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>My entire collection, Cabochon style</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woe1ytn4nute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1jvahhi</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Does anyone have a crème or crelly dupe for this Polish</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxghb7fb9ute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1jvb6jq</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>DIY’d my own polish color. Eep</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvb6jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1jvc78h</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Got a professional manicure for the first time in years, the good, bad, and the ugly</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvc78h/got_a_professional_manicure_for_the_first_time_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1jvbzjd</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Favorite deep purples</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvbzjd/favorite_deep_purples/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1jvbz68</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>You’re A Gem 💎</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvbz68</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1jvbqkl</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>First time posting!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvbqkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1jvblub</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Updating my old mani</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9gh93yfhute1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1jvbdvs</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Dazzle Dry mani lasts only 3-4 days before chipping. How to fix?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvbdvs/dazzle_dry_mani_lasts_only_34_days_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1jvb9cj</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Springtime and first LynB</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvb9cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1jvasal</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Refreshed nails 💅</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvasal</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1jvarbl</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>I bought this thermal in 2019 and it still works!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6az03fabbute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1jv8a6z</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>HELP!!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jv8a6z/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1jv9brn</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Tracking Spreadsheet?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jv9brn/tracking_spreadsheet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1jv96e0</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Show off your most disliked manicures. The ones that made you realise that you hate certain combos/colours/finishes.</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hk5rt96rztte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1jv8qyd</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>When two titans meet</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv8qyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1jv8nx6</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Spring blossoms 🌸</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv8nx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1jv7lkc</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>🍋Lemons🍋</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv7lkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1jv7aza</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>TFW you finally get your hands on your ISO 🥹</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xc965esvltte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1jv6jc4</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Update: got my polish to match the swatch</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv6jc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1jv5y6c</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Nail polish unpopular opinions</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jv5y6c/nail_polish_unpopular_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1jv4rn1</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>ILNP - After Hours (velvetized) 🌃</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv4rn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1jv4p56</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>The Many Faces of Bill</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n60d795f0tte1</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1jv3zg6</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Obsessed with this multichrome from I-Scream Nails. Or should I say Mega Chrome?!</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv3zg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1jvj57o</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Please tell me you know what theme this is</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvj57o</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1jvp73g</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Jaws!</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8ltztbtmxte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1jvo8g9</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>When your wife love your nails</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl50f74xcxte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1jvmk68</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Chocolate Nails</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvmk68</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1jvmcde</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tye8owtuwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1jvmbke</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Inspired by my favorite series made by my best friend fk nails💖</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0maw0hmuwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1jvluy8</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Help:)</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57cowyn9qwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1jvik6j</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Snail nails!!!! 🐌</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvik6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1jvhqv6</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Easter nails 😂🔪</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aim3atksqvte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1jvgduq</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Tried to do a Tortise Shell print, what do you think?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvgduq</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1jvczoy</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Lauren Tsai inspired nails 💅</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu0ouqyarute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1jvcr5g</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Moody Celestial</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gle7rifkpute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1jvclnc</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Would you guys wear these?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21x5gsvhoute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1jvbecp</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Did these myself, what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awolog4yfute1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1jv9ve9</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>I did my sisters nails (1st pic) and my nails.</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv9ve9</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1jv8g62</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>frog nails frog nails frog nails</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddloi2keutte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1jv7nj9</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Dream set, lowkey!!!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv7nj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1jv6tlh</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Simple polka dot look!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv6tlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1jv45k7</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Y2K Fairytale Cyberpunk Dream🦋</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jv45k7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr 11 08:11:46 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_13.xlsx
+++ b/data/collected_data/2025_04_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C876"/>
+  <dimension ref="A1:C1049"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15325,6 +15325,2947 @@
         </is>
       </c>
     </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1jwkq9x</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Made my first press-on</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwkq9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1jwk43m</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>New set 🐍🩸</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00yecjerq5ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1jwk0ta</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>showing off my pink floral nails, not perfect, i’m still learning</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87tuv32mp5ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1jwjxr9</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Summer Nails🌺</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwjxr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1jwjwoq</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>First time getting my nails done</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96vsvjv2o5ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1jwj4ai</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Just got my nails done in Tokyo!✴︎⭐︎✴︎</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzjvilkxd5ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1jwioqu</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Day 1 of trying to heal my nails!</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwioqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1jwikm2</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Share your not-so-great nail experiences</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwikm2/share_your_notsogreat_nail_experiences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1jwiia1</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>🐚🌊🏝️</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bogqhthd65ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1jwibfv</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>How much do they give it from 1 to 10?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wvscfw345ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1jwi3a0</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Gel polish chipped &amp; peeled at cuticle area after a day. Reasonable to ask salon to redo this nail?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1spi4qg15ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1jwg9b1</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Strawberry Theme for April!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwg9b1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1jwgl3s</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Tips to fix this so I don’t suffer</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3z6dlngl4ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1jwgqso</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>How do you type with long nails</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwgqso/how_do_you_type_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1jwfz6b</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Pain From Nail Polish?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwfz6b/pain_from_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1jwhsmy</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>I need to find a gel nail polish brand that’s cheap and easy to get in both Vietnam and USA.  Super urgent. Please help with any advice!!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwhsmy/i_need_to_find_a_gel_nail_polish_brand_thats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1jwhjo5</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>nails I did today and they turned out very pretty💜</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwhjo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1jwh7y9</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Do you prefer with or without rhinestones? I love them</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjep309vr4ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1jwfzam</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Gel manicure of the week ⭐️</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dep0vnthf4ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1jwfd9c</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>How do you remove Gel X nails?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwfd9c/how_do_you_remove_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1jwfbh3</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Jack @serenitynails on IG gets me right every time 🥹</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwfbh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1jwfvff</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Thoughts on this black effect ?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyjfx5nfe4ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1jwf4v1</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>First Polygel Set!</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d6kdf5w874ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1jwe9h8</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Spring Set</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9scqlm1z3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1jwe7mc</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Do you tip at home nail techs? Why or why not?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwe7mc/do_you_tip_at_home_nail_techs_why_or_why_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1jwe4mc</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>April Easter Nails🥕🐰🐣🐇</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwe4mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1jwe29q</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>🌷Spring Nails🌷</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frhlymh5x3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1jwe050</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>I think I messed UP my friend's nails</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwe050/i_think_i_messed_up_my_friends_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1jwdrgz</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>did some Kirby &amp; Waddle Dee nails on myself 🤭</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwdrgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1jwdlu2</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Pink sparkly nails 💅</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwdlu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1jwdkix</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>I love when my husband does my nails</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aveqga3ls3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1jwdiuo</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Strawberry Season 🍓</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwdiuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1jwd6ok</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>builder gel set</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwd6ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1jwcxim</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Why do cuticle nippers come with little clear balls?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwcxim</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1jwcsbh</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>the healing power of nail art</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz5yet8al3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1jwcnv1</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Did these today, husband said it reminds him of the Monet on the last slide.</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwcnv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1jwccjh</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Easter set!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnno5endh3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1jwc9cy</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Which shape?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwc9cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1jwbhz6</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>first manicure in 3 years!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ap3hs1gx93ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1jwbw43</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Advice for my cuticles after my tech butchered me😭</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/or4qq2bbd3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1jwbxdn</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>classic french</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbtg7xomd3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1jwbmi8</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Do nail artists do a bad job on purpose to keep you from coming back?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwbmi8/do_nail_artists_do_a_bad_job_on_purpose_to_keep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1jwa09f</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Why do my nails keep chipping?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8pt43ysx2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1jwb8ul</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>First time posting here. I got these nails done for my birthday 💕</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwb8ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1jwb6md</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Bite nails</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwb6md/bite_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1jwavjo</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Do these look right?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwavjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1jwb95v</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59teuflu73ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1jwb7wv</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Nail help!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwb7wv/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1jwb4oc</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>First time posting. Here’s my Easter set 🦋</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwb4oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1jwarsg</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Handmade</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwarsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1jwar2s</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Easter Nails 🐰🌸💅🏼</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwar2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1jwajdi</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>How often do you go to the nail salon?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwajdi/how_often_do_you_go_to_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1jwa6az</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Natural nails with rubber base and French design ;) The cut is my fault but other than that what do you think?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwa6az</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1jwa15t</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Anybody else have a “comfort” go to style?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwa15t/anybody_else_have_a_comfort_go_to_style/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1jw9x2y</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Love the chrome</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw9x2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1jw9t90</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>New set 🫐😊</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw9t90</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1jw9cw8</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Reasonable price?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jynt4klms2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1jw92ig</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Mini Egg /Easter set 🐣</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw92ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1jw8w39</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>The vision vs the execution</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw8w39</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1jw8o5z</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Fav nail set ever</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/217fq3nfn2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1jw8nw8</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Chromed blue ombre</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goczn5sdn2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1jw8kg0</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I used gel polish for the first time!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw8kg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1jw8anm</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Galaxy esq nails ✨️</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8q1acdyhk2ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1jw81se</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>My newest set 🐚🩷</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d1v0hdoi2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1jw7php</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Cat eye with chrome tips ✨</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98lgc7g5g2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1jw7enq</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>How does this nude look with my skin tone? Is it too peachy/pink? Do I have yellow undertones?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu9vf4eyd2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1jw7bwa</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Bunny nails</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw7bwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1jw79yp</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>I asked ChatGPT what nails I should do next and this is how it turned out</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw79yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1jw6iqo</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>First time w nails done in like 8 years</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw6iqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1jw5x7t</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>had a few breaks so this months shorties! ☁️ my nails by @carlasnailcreations</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/momxuisy22ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1jw5rv0</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>New nails today</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jldhaiw12ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1jw5mss</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>first time posting here, what do we think?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pftmhk8t02ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1jw58pt</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>AN ALMOND SHAPED RUSSIAN GEL MANI IN A MILKY BABY PINK 🤍 🩰</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmi182awx1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1jw4trr</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Not sure about this color on my skin tone</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7r5aizltu1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1jw4r2w</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Help!  Milky white pink gel manicure - tip edge turning dark/black</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jw4r2w/help_milky_white_pink_gel_manicure_tip_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1jw4lhd</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Trying out 3d gel, loving textured nails more than I thought I would</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw4lhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1jw4jcu</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Spring purple!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbebhgzps1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1jw4b9e</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>First set!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7uh2sj4r1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1jw4anm</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Obsessed with my spring nails!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9jxsd50r1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1jw3cox</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Help me Nail Sleuths! (Gel polish Colormatch)</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jw3cox/help_me_nail_sleuths_gel_polish_colormatch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1jw43uz</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>It feels like fall in PA</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebkl3bcmp1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1jw426o</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>My nail tech never disappoints</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9mii3e5p1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1jw3p4n</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Easter Eggs and Peace on Earth for all - Mood</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw3p4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1jw3fia</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>i did these myself today. what do you think?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2qzypwok1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1jw3c1f</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Just refreshed my neon pink hair and figured I’d get my newest set to match 🩷</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw3c1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1jw2ujx</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Back at it again</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw2ujx</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1jw2sdp</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I did my nails! Rate?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jw2sdp/i_did_my_nails_rate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1jw2n8o</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Best nails I ever had !</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3vt1apqwe1ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1jw2ctx</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Home solution to removing acrylic gel nails? Unhinged ideas needed</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jw2ctx/home_solution_to_removing_acrylic_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1jw1o8x</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I have a Gel allergy from the salon, does anyone know if soft gel press on nails would also give me a reaction?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exg9n9hm71ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1jw1d2w</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Best UV Nail Lamp? Need one that doesn't suck pls</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jw1d2w/best_uv_nail_lamp_need_one_that_doesnt_suck_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1jw1idz</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>New mani☺️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw1idz</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1jw0tui</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Soft Gel. 🧡 Encapsulated Design, orange chrome and lines 🍂✨️🙌🏼</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw0tui</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1jvtfl2</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Tried the stained glass inspo with cat eye 😍✨</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv3s0adq3zte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1jvwmf6</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Nail stick-on strip recommendations?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvwmf6/nail_stickon_strip_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1jvwrd5</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Struggling to apply acrylic press-ons with flat-ish nail beds - gel glue, uv lamp.</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jvwrd5/struggling_to_apply_acrylic_pressons_with_flatish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1jw0llf</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Tips on Gel Nail extensions</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw0llf</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1jw08hp</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Pink Florals</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7fs0gosw0ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1jw05nk</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Matte vines</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw05nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1jvxsvw</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Nails inspired by one of the traditions of my country called "painted eggs" for the upcoming Orthodox Easter</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvxsvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1jwk8wj</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Miss Frankie is getting cranky because bedtime was HOURS AGO, how dare I still be on this shi- 😂</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwk8wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1jwjy64</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Sinful Colors 24/7 (920)</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwjy64</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1jwjhfp</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>How do I not change my polish?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwjhfp/how_do_i_not_change_my_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1jwiilg</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Lush ft. Jammy</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwiilg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1jwi28b</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Panic buying</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hw17hse515ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1jwhthq</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>A little experiment</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n7ofnfldy4ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1jwhhac</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>The wargaming people have discovered nail stamping</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwhhac</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1jwg1g6</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Dip powders?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwg1g6/dip_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1jwg0wt</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Antique silver and bronze</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwg0wt/antique_silver_and_bronze/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1jwfq9f</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Drying drops</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwfq9f/drying_drops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1jwf7at</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>anxious about work so added an evil eye to my manicure</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwf7at</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1jwf70z</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Been wearing polish for half a year now and I just got my first compliment from a stranger today! No one irl cares so I just had to share it with you all 🥲</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bogbf9fu74ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1jwdbsj</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Acetone vs non acetone</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwdbsj/acetone_vs_non_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1jwdbpa</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Oil painting design on nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwdbpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1jwd8bz</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Tried to make it hideous but honestly I kinda love it</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwd8bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1jwd6im</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Best (non Maniology) top coat for stamping?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nube077yo3ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1jwcpd4</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Glitter grabber not working?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwcpd4/glitter_grabber_not_working/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1jwblar</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Rock bottom</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwblar</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1jwalx1</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Dazzle Dry collection</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwalx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1jwalpw</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>ilnp - Winter Dream</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78vwn3gj23ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1jwaiam</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Original OPI Less is Norse (from 2017)</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwaiam/original_opi_less_is_norse_from_2017/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1jw7rce</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Good replacement for sinful colors?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jw7rce/good_replacement_for_sinful_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1jwa405</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>HELP with Acrylic Nail Instructions to Professional</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwa405/help_with_acrylic_nail_instructions_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1jw9ssn</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Kate Middleton nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw9ssn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1jw9cxe</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Spring Crelly-Flakie Skittle</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw9cxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1jw933t</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>DAE ever change their glossy manicure to matte after a few days?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw933t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1jw8xqo</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>I’m Beautiful. I’m Mad. I’m Obsessed.</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/35nd7l3fp2ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1jw8xll</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Dear Makers, Please make a polish/collection to encapsulate our collective anger, confusion, anxiety, etc at the chaos 1 person can do.</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jw8xll/dear_makers_please_make_a_polishcollection_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1jw8gqw</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Dam top coat reviews?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jw8gqw/dam_top_coat_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1jw8dcf</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Looking for a specific color (photo)</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0v7hfw14l2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1jw85u9</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Trying out some new old techniques.</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw85u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1jw6gqi</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Lemon Lime Fizz</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nl8pa1272ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1jw52os</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>The Powerhouse of The Cell</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw52os</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1jw4bno</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Enamel hardener</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jw4bno/enamel_hardener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1jw4ar9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>A new glowy combo with colors I already had</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw4ar9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1jw46x3</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>ILNP FTW</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw46x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1jw3p6w</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Toppers are my lifesaver</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qw9bcimm1ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1jw36qh</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>I did the new magnet thing 🧲💘</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw36qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1jw0wq2</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>HELP… which nude polish would suit my skintone?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw0wq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1jw2s6e</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Witchy green vibin'</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4szra5mzcwte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1jw2gm4</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Beautiful sibling</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw2gm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1jw2dzb</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>To all professional laquerisras (polish makers, artists, etc)</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jw2dzb/to_all_professional_laquerisras_polish_makers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1jw1he2</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I do enjoy a unique blue!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw1he2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1jw1fhy</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>ILNP Pitter Patter ☔️</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw1fhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1jw1aln</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Lux</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw1aln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1jw19kj</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>BKL's tariff statements</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw19kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1jw0zd5</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>stage mani for my first time in front of a mic in years 🤩</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw0zd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1jw06is</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>BKL: The Blade of the Frontiers</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jw06is</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1jvzutq</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>From Royla Lee (formally Wildflower Lacquer)</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvzutq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1jvzp8e</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Snack Matching</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llf8utlqs0ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1jvyxuh</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Why do my nails do this?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvyxuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1jvypu8</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>I’m obsessed 🤩😍</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvypu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1jvylhm</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Needless to say, my dog was not impressed</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvylhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1jvx07u</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Found the perfect background for my photo...</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hk7x7rb370ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1jvwdaa</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Confetti charm nails</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9os190410ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1jvu8jq</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jvu8jq/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1jvu4hh</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Used my new dollar store find and mixed a gradient &lt;3</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvu4hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1jvsz93</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Still in love ♡ ( but with better lighting and focus)</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtebj0okxyte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1jwhorp</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>today's nail art✨💛</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwhorp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1jwgaoo</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>coachella nails</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwgaoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1jwfxky</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Lil peep inspired nails I did</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0o3vy20f4ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1jwfcof</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Our clients are Spring Ready ✨🌸</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwfcof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1jwcvxp</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Golden Waves</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwcvxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1jwc02x</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>It’s time for neon nails!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwc02x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1jw8r8j</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Silicone hand</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/800g3vrzn2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1jw8q77</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Chromed blue ombre 💙🩵</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzff0awtn2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1jw842r</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>My nail artist @nails_emmywynn never misses and I love the details on this set 🐚😍</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ijee2b5j2ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1jw0pg2</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Nail Charm Product ID?!</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5edex4901ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1jvvasx</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Mushroom Nails</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82ufhy4bqzte1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1jvyuku</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Spring nails 🌷🌼</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvyuku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1jvw9kq</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Easter nails from concept to execution</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cplvlj6400ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1jvuudk</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Pink and green freestyle</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvuudk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1jvtq5d</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Suitable for summer?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jvtq5d</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr 12 08:10:19 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_13.xlsx
+++ b/data/collected_data/2025_04_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1049"/>
+  <dimension ref="A1:C1222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18266,6 +18266,2947 @@
         </is>
       </c>
     </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1jxc3lk</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>maintaining nail length</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jxc3lk/maintaining_nail_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1jxbylg</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>hey! i have just started doing my own nails and wanted to share🥰 any advice would be really appreciated! i'm just winging it at this point 🍀</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxbylg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1jx5zmr</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Prom Nails!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66n06t9w3bue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1jx77mg</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx77mg/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1jx8etf</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Spring Nails (w/ real flowers) from Korea!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx8etf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1jx99a3</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Cat eye again!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgq4xs6g1cue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1jxa8fc</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Just wanted to show off my nails for inspo!</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxa8fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1jxas6n</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>momsomnia manicure</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghh8d7p5jcue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1jxaiye</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Current Set. Alien Vibes.</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxaiye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1jxaez2</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Recent press-ons!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxaez2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1jx9xrj</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>I’m stumped. I keep getting this small sliver of a nail growing on the left side of the proper nail. It keeps coming back even after I trim it and has been for the last few months. Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4lw3co29cue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1jx9tmh</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Monkey nail</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx60e42r7cue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1jx9jfx</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>What length of nail do you think I should choose? I want them to last a long time</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx9jfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1jx9hrh</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>What would be the best way to apply Etsy press ons?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx9hrh/what_would_be_the_best_way_to_apply_etsy_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1jx9hei</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Monomer on carpet?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx9hei/monomer_on_carpet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1jx9epa</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Groovy spring nails</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zujddi33cue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1jx97jh</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>how is it</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6fl8gm0w0cue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1jx93xy</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Swan Nails 🦢</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq11jfntzbue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1jx91p6</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Jewelry nails</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx91p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1jx9161</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Has anyone used up an entire bottle of gel polish when DIY? How long did it take?</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx9161/has_anyone_used_up_an_entire_bottle_of_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1jx8ugp</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Trying to grow my nails out.</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx8ugp/trying_to_grow_my_nails_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1jx7m9j</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>My attempt at Easter nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx7m9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1jx779g</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Spring/Easter Nail Art 🐣🩵🩷</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx779g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1jx74wy</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>90's vibes ✨🩷🌈🏁</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wd11lqd7fbue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1jx72qm</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Custom set I made for my bestie.</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsvmx2klebue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1jx6wml</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Second Spring set</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx6wml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1jx6rh5</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Hi everyone I use to be just a follower on this page until…</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx6rh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1jx6ec0</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>jhope concert nails!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29qwtgpu7bue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1jx66wa</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Can you never take a break from gel x?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx66wa/can_you_never_take_a_break_from_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1jx66q5</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>My current set, and my last set</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx66q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1jx5vzx</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Can this be fixed?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz0cjmyv2bue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1jx5nmj</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>cherries</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lajxmann0bue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1jx5mj7</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Was this a bad color choice? Was trying for a natural jade look</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncth4x4d0bue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1jx5jq9</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>The most basic black nails lol</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqywsaemzaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1jx566p</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Cuticle care help</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx566p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1jx5grv</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Almost done with nail School!</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbcau34vyaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1jx5agq</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I’m obsessed with the cat eye</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx5agq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1jx4s7w</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Champagne Cat Eye Gel</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci09oebisaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1jx4ka6</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Did stained glass cat eye today..</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx4ka6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1jx4h2x</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Hoppy Easter (almost) 🐰</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1dygrympaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1jx40x6</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Handmade Press On Nails Recommendations</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx40x6/handmade_press_on_nails_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1jx405n</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Bee nails!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kylryctblaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1jx3yco</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>What shape is this</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw0zrr5ikaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1jx3gia</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>What is this white on my nails by the tip?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx3gia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1jx32rg</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Advice??</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx32rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1jx3asb</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>💗I love sparkles💗</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cwj77ro2faue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1jx396k</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>My sister in laws work</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0u15d8qeaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1jx3811</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Tried UV gel polish!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx3811</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1jx37td</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>I know long nails aren’t popular, but I have another nail post😂</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fz2iugdeeaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1jx316e</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Nails for Easter  💅🏼 🐣 🐰</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5zaz0ltcaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1jx2yd5</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>thoughts on the color of my nails?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r37fmxt5caue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1jx1vmv</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Set 2 - Butterfly wings🦋</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx1vmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1jx1wh2</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Where can I find an LED only nail curing lamp?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx1wh2/where_can_i_find_an_led_only_nail_curing_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1jx2amd</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I don’t which shape looks better on me. Help me choose</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx2amd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1jx2khk</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Told my tech ‘Floral, Feminine, Dainty, no orange’ 😍</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9avuqex8aue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1jx2cek</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Just got hard gel extensions for the first time!</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx2cek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1jx1zo2</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Simple ombre</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7poit174aue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1jx1y95</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>💚🩷 Garden Path Lacquers Verdant 🌵 My first GPL purchase. Amazing formula and shimmer! ✨</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx1y95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1jx1hxi</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>What’s wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx1hxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1jx1dkv</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Four weeks of growth and four hours of work. First time using rubber base, I'm still slow but I like the end result.</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx1dkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1jx0nh9</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>❤️‍🔥 the gold chain is my favorite part</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx0nh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1jx0ju9</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>is it bad?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx0ju9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1jx0i38</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Advice for my nan who is</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jx0i38/advice_for_my_nan_who_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1jx0f82</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Advice needed, do these look outdated?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx0f82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1jx065z</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Milky Sparkle</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nav6passp9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1jx0alr</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Looking for a good quality UV kit</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1b4foarq9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1jwzypx</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Spring ☺️💛</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwzypx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1jwzure</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Will I ever get over cat eye polish? No. No I will not :)</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdbies3cn9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1jwzq4p</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Tried to do a Russian mani on myself…. Love how this color looks like I have a subtle French tip 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwzq4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1jwzngr</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Set I did on my cousin today!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwzngr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1jwzlrg</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>vacation set 💜💚</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhn3letgl9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1jwzl1h</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>New Nails☆</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rfj86kbl9ue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1jwzies</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>I love this ombre</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f1wznxrk9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1jwz07h</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>nail shape help!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwz07h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1jwxyyi</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>How do you make nail press ons last?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwxyyi/how_do_you_make_nail_press_ons_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1jwy2nu</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My nails, I love the design and most of the nails are natural hehe they think?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1unjxcxs99ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1jwxy3x</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>First set after a while</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwxy3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1jwxq44</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Found in my camera roll and had to share!</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwxq44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1jwui6g</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Is it normal for my cuticle to be so red and bleeding after hard gel manicure</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwui6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1jwxc42</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>🐰Happy Easter🐰</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys4jui5949ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1jwwqev</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>My nail broke 😩</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1zjefhpz8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1jwwdry</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>simple spring 🐇🌷✨</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwwdry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1jwvywv</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>First time having my nails done - a few questions (nail inspiration art by dvok_official on IG)</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwvywv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1jwuzqt</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Cateye butterflies are so cool</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwuzqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1jwtejq</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Peep inspired nails</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwtejq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1jwpjg0</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Airbrushed nails.</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwpjg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1jwxjyr</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Should I file all the soft gel off</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwxjyr/should_i_file_all_the_soft_gel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1jwxcce</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>First time trying “nail foundation” I really like it! :)</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlgrrmsa49ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1jwwh1b</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>My Mom gave me a manicure 💅 ✨</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwwh1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1jwwgvq</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I was hoping to do spring nails but feel it’s more summer</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwwgvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1jww4yv</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>-90C (-130F) metal vs nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jww4yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1jwvych</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>OPI Cajun Shrimp never disappoints ❤️</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi9dwqoxt8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1jwvmlh</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Feeling good today 💅</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwvmlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1jwvbyy</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Palette</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ddghi6bp8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1jwuokm</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Tried some strawberry nail stickers 🍓⛓️🍓</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dahyzuygk8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1jwuipg</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>A simple look</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwuipg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1jwuf3c</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>something simple and unique</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4ad1nbji8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1jwues6</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Struggling to do french tips at home. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jwues6/struggling_to_do_french_tips_at_home_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1jwu3a6</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>It took 5 hours to make this set🐢🐢</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm93n732g8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1jwtcx7</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwtcx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1jxayvk</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Unpopular opinion: please for the love of god, can we move on from brown bases with green/blue/pink shimmer? Dust to dust, ashes to ashes, I am bored to DEATH of this trend 💀</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jxayvk/unpopular_opinion_please_for_the_love_of_god_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1jxasv3</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Blueberry Nails 🫐</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxasv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1jx8srx</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Any nail companies having any sales coming up soon?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jx8srx/any_nail_companies_having_any_sales_coming_up_soon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1jx8dqs</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>FeelingSpringy!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx8dqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1jx6suh</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Atomic has 40% off sale on discontinued polishes</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atdc7iutbbue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1jx622r</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Starrily Red Jellies</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jx622r/starrily_red_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1jx53se</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Demogorgeous</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq6gotxnuaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1jx44po</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>DIY manicure!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu3kld6gmaue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1jx3ulw</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>anyone else not able to use a glass file??</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jx3ulw/anyone_else_not_able_to_use_a_glass_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1jx3nlt</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Painted my nails for my friend’s baby shower 💖</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx3nlt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1jx28uw</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Desi Lacqueristas, hair oil warmers double as nail soaks 🥹</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx28uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1jx1wf4</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>💚🩷 Garden Path Lacquers Verdant 🌵 My first GPL purchase. Amazing formula and shimmer! ✨</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx1wf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1jx1omi</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Lurid's Nettle and Briar</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uf276kj1aue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1jx1nu5</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Strongest Shimmers?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jx1nu5/strongest_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1jx17su</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Duped myself 3 times 😆</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/segxzwyyx9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1jx16sy</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Higher quality dupe for Sally Hansen Sturdy Sapphire color?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx16sy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1jx0l2i</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>I wanted to do floral for spring but I’m not a pastel person</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx0l2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1jx0ka7</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Dragon Darts "suede" nails</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uvx1r09xr9ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1jx01aa</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Another 2019 Thermal that still (kinda) works</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ztka6qqo9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1jwzpd0</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Canadian Brands with Nail / Jojoba Oil?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwzpd0/canadian_brands_with_nail_jojoba_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1jwytxx</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Anybody has space phoenix by fancy gloss?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwytxx/anybody_has_space_phoenix_by_fancy_gloss/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1jwyref</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Magnetic polish wont dry!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwyref/magnetic_polish_wont_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1jwy8lh</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Mini eggs 🪺</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruv0qs62b9ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1jwxlsv</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Is this shrinkage?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwxlsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1jwx76v</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>ILNP Kiss and Tell</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwx76v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1jww55d</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>wasn’t completely sold on my mismatched set so i made it a little less mismatched</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jww55d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1jww41b</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Tell me your fav polishes with a red shift/shimmer</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jww41b/tell_me_your_fav_polishes_with_a_red_shiftshimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1jww26h</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>what have been the responses from mooncat for those whose orders arrived damaged?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jww26h/what_have_been_the_responses_from_mooncat_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1jww1zz</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Lurid Wish List - Help!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jww1zz/lurid_wish_list_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1jwvzuc</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Gelcare Sale</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwvzuc/gelcare_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1jwtb1g</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Comparison request?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwtb1g/comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1jwvc08</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Stolen Kiss ft. Styrofoam</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwvc08</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1jwvb9f</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Ignore dry hands haha</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwvb9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1jwv2gb</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Liquid chrome?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.beyondpolish.com/products/londontown-lakur-enhanced-colour-chrome-glaze-aurora-0-4-oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1jwuvmh</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Help me find a good shade to match my girl!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwuvmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1jwulfa</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Loving this flashy pink</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwulfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1jwudas</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Can builder gel help/work with nail that has significant pits and ridges?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwudas/can_builder_gel_helpwork_with_nail_that_has/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1jwtrlz</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>She wore an itsy bitsy teeny weeny…</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f64xvkcld8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1jwtik4</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Looking for a simple solution to bending, peeling nails 🙏</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwtik4/looking_for_a_simple_solution_to_bending_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1jwtf17</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Beautifully packaged cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ckwpbf1b8ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1jwstpx</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Deep space 🌌</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uy20n88m68ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1jwst59</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>I hate how Joker has put so many people off this beautiful colour combo. Purple and green Manis are perfect for spring!</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wp5yrxh68ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1jwsle5</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Espress-oh!🔬☕️💜🩷</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwsle5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1jwsck2</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Finally going to get a magnet 🧲 which one is best?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jwsck2/finally_going_to_get_a_magnet_which_one_is_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1jwsac4</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>💎🩵Aqua Geode🩵💎</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwsac4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1jws6gh</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>There was an attempt</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jws6gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1jws5fn</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>My nails are short and stubby, and I've been recommended to try gel-x extensions. Is this sort of look possible?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w89hh4qh18ue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1jwrrrv</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Snake</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwrrrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1jwretb</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Periwinkle is so dreamy ✨</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ntqappz6v7ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1jwqx1y</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>similar, but differnt</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwqx1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1jwqrst</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>What nail shape is best for my long/chubby fingers?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmvzpgttq7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1jwqqtb</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Mondrian</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9skgvdulq7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1jwqjsx</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Spacey nails 🌌</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2uwlyk4p7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1jwp3jl</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>So... what does Essie Play Date actually look like?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84rga91zb7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1jwp0cp</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Can I offer you a fugly muck in these trying times?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq4vomzcc7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1jwmrmy</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>We've had a few casualties while fencing</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwmrmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1jwm4ig</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>An ocean-themed mani inspired by my friend's coastal wedding this week</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwm4ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1jxb1qh</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Is it too pink?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppjz3bmemcue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1jx9lan</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Monkey nails</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gynu04c45cue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1jx90j1</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Another beginner set. What do we think? How can I improve on nail art??? Be nice pls :p</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx90j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1jx6k38</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>a simpler design 😍 but I think it's very pretty 🥰 do you like elegant or more colorful designs? *The design was taken from the internet, the client brought it to me and we recreated it🫶🏼*</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja9uq4sf9bue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1jx0kmt</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Gifts for my sister</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jx0kmt/gifts_for_my_sister/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1jx0et1</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>How to accomplish this?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jx0et1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1jx03rk</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Aurora Glaze✨</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vk7ouc03p9ue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1jwo2pp</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Colorful Spring Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://youtu.be/DO2iH45_fxM?si=tjGbwCfzJG4H2Uly&amp;t=26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1jwvpjr</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Did my best with gel!</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwvpjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1jwv0pt</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Cat eye butterflies</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwv0pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1jwucdg</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Recent practice</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jwucdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1jwsxtw</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Sailor Moon inspired</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv2e8inh68ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1jws738</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>April Easter Nails🥕🐰🐣🐇</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jws738</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1jws5fo</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Easter mani 💅🐰</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jws5fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1jwrda6</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Are they yummy</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4myivbhv7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1jwqxic</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Mondrian</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43tqcod3s7ue1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr 13 08:10:24 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_13.xlsx
+++ b/data/collected_data/2025_04_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1222"/>
+  <dimension ref="A1:C1401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21207,6 +21207,3049 @@
         </is>
       </c>
     </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1jy2hcm</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>The work of my girlfriend, due to low karma she couldn’t post</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy2hcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1jy2csi</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>I did it by myself!</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy2csi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1jy2cod</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>First time trying something that isn’t cat eye 😍</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy2cod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1jy2c9i</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I just did my own nails and then i ruined my own nails</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy2c9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1jy27ya</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Stubbed my toe</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jy27ya/stubbed_my_toe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1jy24he</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Nails i did today (:</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy24he</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1jy0znz</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Any tips for growing back nail?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jy0znz/any_tips_for_growing_back_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1jy1slk</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>are these acceptable for a professional manicure? 🫠</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy1slk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1jy1plw</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Showing off my new set from today</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy1plw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1jy1i4s</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>DIY dip powder nails. Reminds me of strawberry milk. 🍓🐄</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m0i9m6kasjue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1jy16c7</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy16c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1jy11w0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Lilac biab</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy11w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1jy0v2y</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>New to the DIY nails.</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy0v2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1jy0ntf</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>simple, yet festive🐰✨</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy0ntf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1jy0mqi</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Nails I did today</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avqk1vmkhjue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1jy0jgs</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>What do we think of the new set?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bqxti1igjue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1jy0eq7</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>🌅 Sunset and palms🌴</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy0eq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1jy0aca</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>So proud</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy0aca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1jy09lp</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Alice in Wonderland Nails</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy09lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1jxztxz</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>new artist</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o4r7gn08jue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1jxzfg5</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>One piece nails 💜</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxzfg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1jxy6hh</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Guys 😭</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/342z5ntvpiue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1jxy41n</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Tried a pink polish for the first time and... I kinda love it!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxy41n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1jxxk2a</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Pretty new set 🎀</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro6vy46ejiue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1jxx2nb</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Yellow Vibes 💛</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upv707qjeiue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1jxtzs4</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>is this a bruise or fungus?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxtzs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1jxwstq</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>New set for Easter 🥰</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v66svfrqbiue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1jxtbzf</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>How do you do your household chores with manicured nails?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jxtbzf/how_do_you_do_your_household_chores_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1jxwdzm</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxwdzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1jxvz5c</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Fresh mani !</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emc4ht3f3iue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1jxvxoa</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>First nail appointment in 5 years</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwujg3k03iue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1jxvmt8</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Advice please!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvmt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1jxvdkb</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Easter Nails!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvdkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1jxvbtq</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>New nail artist!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvbtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1jxuym0</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Need some help!</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsh1z6kjthue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1jxulk4</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>my wonderful friend did ma nails!!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxulk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1jxuk8j</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Nails I've done in the past weeks</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxuk8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1jxuiqs</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxuiqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1jxuflf</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Love them so much🩷</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxuflf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1jxu2y5</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>my new (favorite of all time) set</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxu2y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1jxtux7</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Love giving my nail tech full creative control</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxtux7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1jxtt9s</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>First time using blooming gel</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxtt9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1jxtdww</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Possible getting engaged, which nail paint looks good?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxtdww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1jxtat6</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Next Appt Isn’t Soon Enough 😭</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxball0dehue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1jxsq11</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Any tips on how to have healthy strong nails?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxsq11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1jxt1xf</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>New set I did</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bnijsw5chue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1jxsxdn</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Porcelain mask nails!! Hand painted by me. &lt;3</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugecfzi2bhue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1jxso9v</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Nail Salon Pricing</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2jd0sxv8hue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1jxsa2l</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Men getting mani/pedi</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jxsa2l/men_getting_manipedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1jxs3cz</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Are my nails long enough for acrylics/extensions?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze17136u3hue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1jxrpf7</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>First time getting gel nails</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2uuyebp0hue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1jxrix3</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>My first time doing press on nails</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxrix3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1jxrfow</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>First time having short nails🌷</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3paxifgfygue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1jxr9dt</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>My lady had an off day</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekpsneq0xgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1jxr12w</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>How do you feel about orange nails?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kk23hvzugue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1jxqvj1</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Removed acrylics, what will help?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/laosbujvtgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1jxqudz</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edi4e22mtgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1jxqmny</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>color change?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://media.discordapp.net/attachments/1343044712784990320/1360650190004027504/IMG_0749.jpg?ex=67fbe3bc&amp;is=67fa923c&amp;hm=0b7e02a408c6dca9d638117e4de623010b6a0d5a8536c3c3d36d901196a0d073&amp;ink</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1jxqjf4</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Took some inspo from this sub...</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c54j5a1rgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1jxr0fo</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Trying out some simple press ons</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxr0fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1jxqixa</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>why does my nail split like this</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umykv44xqgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1jxqcxt</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Sabrina Carpenter inspired nails (I did these myself)</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxqcxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1jxqzhi</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Flowers !!!😊</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh8n6exrugue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1jxqtep</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Is there any way to combat the dryness I’ve been having in my nails lately?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s32n134etgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1jxqa2l</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Help! Which electric nail file is actually good quality?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jxqa2l/help_which_electric_nail_file_is_actually_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1jxq88a</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>First time doing nail art</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbg1r0jgogue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1jxq4ug</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Spring 🥚🥚</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxq4ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1jxpa0r</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Am I being too Virgo or is this just a messy acrylic set?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxpa0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1jxpwf4</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Very out of my comfort zone</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ph4vftrlgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1jxpqfe</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>I love my nail tech so much</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvcrx4rekgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1jxp0d7</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>3d nail designs i’ve done recently! obsessed with cake nail designs lately!!🧁💕 all hand sculpted by me 🩵</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxp0d7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1jxoyqz</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Cracked big toe keeps cracking</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jxoyqz/cracked_big_toe_keeps_cracking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1jxox76</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My birthday set 🖤 Mani by me, pedi at a salon✨</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8nuo8hydgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1jxda0k</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Nail Growth Progress</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxda0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1jxdgfv</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Why does my nail grow like this?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxxbb9irhdue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1jxeb5t</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Finally went for a set that’s been on my Pinterest board forever.</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rgb3kg0tdue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1jxfyzu</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Spring Garden inspired</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxfyzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1jxglbl</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>What is the best nail shape for me?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxglbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1jxhx8n</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>apex??</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29fv3rr1ueue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1jxjvp4</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Contact dermatitis or bad cuticles</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxjvp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1jxonuu</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Spring/Summer Nail Palette</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2aykhpyybgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1jxoatj</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>tell me these aren’t the cutest spring nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsktg3629gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1jxo7gc</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>I got my nails done today!!</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cggkpbya8gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1jxo2zg</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Spring 😍</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l03p3g1b7gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1jxnnr1</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>How’d they do?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxnnr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1jxnnea</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Loving the clean/abstract aesthetic ❤️</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s9exqbv3gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1jxnfsy</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>I am doing my gel’s tomorrow</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jxnfsy/i_am_doing_my_gels_tomorrow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1jxn7uq</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Spent $$$ on these elegant, coffin-shaped claws and this woman zoomed in on the cat hair on my thigh like it was a CSI crime scene. Ma’am. Focus on the glam, not the fur. 🤣</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/39rxlhvh0gue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1jxn762</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Some of my fav nails ever!!!</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxn762</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1jxmvql</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Simple Spring nails 💜</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxmvql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1jxmitx</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Cadillacquer - The Quiet Chaos</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxmitx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1jxmfr0</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Yet another fishing lure mani 🎣</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6lx9oemcufue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1jxlj7a</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Speckled</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yijziednfue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1jxlgj2</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Some sets I’ve gotten through the years</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxlgj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1jxlbbc</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Kiss press ons have saved my wallet 😂</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkewe8zklfue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1jxkrxn</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Easter skittle</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1mdsypbhfue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1jxkrpl</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Strawberry nails!</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxkrpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1jxkagl</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>April nails</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4i14o9jdfue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1jxk8jw</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Semi-permanent enamel 🤍</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in5muxp3dfue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1jxk8c2</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>the perfect red 🩸✨</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mapdae22dfue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1jy2pg0</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>My mum nailed my birthday gift last year</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jy2pg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1jxvrg7</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>vibe of peace</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tnwskoc1iue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1jy03ov</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Is this normal for gelx?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jy03ov/is_this_normal_for_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1jy01om</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Looking for copper/bronze polishes</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jy01om/looking_for_copperbronze_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1jxzd9z</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>De-Influence me??</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yh2xrjij2jue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1jxy2h6</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>5 very slightly different pinks</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxy2h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1jxy10f</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Please help me find this color in a different brand</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxy10f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1jxxfge</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>So sparkly ✨</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxxfge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1jxxep2</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>no illusions</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nh31bh0whiue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1jxxdcd</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Eternal Forces from EdM is breathtaking</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxxdcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1jxxaov</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Attempt at Porcelain nail art</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxxaov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1jxwrf0</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>🧲 🌟experiment…successful?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4b9zfukcbiue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1jxvxtq</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>First purchase from cracked. How are these picks?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvxtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1jxvr8t</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Love or hate?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvr8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1jxvgec</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>I invoke thee 🔮</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvgec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1jxv8a9</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Surprise magnetic alert! Microscopic by Kathleen &amp; Co.</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxv8a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1jxuvy3</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Fairest of Them All \ Lemon</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxuvy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1jxuruo</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Show Me Your Organizers/Displays!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jxuruo/show_me_your_organizersdisplays/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1jxtb54</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Tried the Magnetic “French Manicure” Technique</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6i0b1xfehue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1jxswgi</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Got a little too file happy 😆</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxswgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1jxrydd</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Got 20 cabochons as a test and my inner magpie is cawing with joy!</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxrydd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1jxrwmf</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Blue Sky Gradient</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxrwmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1jxrmvb</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Such a simple look, but I really loved this mani! 💫✨</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxrmvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1jxr3kg</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Thermal + Stamping = fancy art nouveau nails</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxr3kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1jxqtdg</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ojzejpdtgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1jxq7hf</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Easter nails</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxq7hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1jxq41u</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Just…every picture I took of Fairy Dust. NBD.</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxq41u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1jxpm4q</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Another round of Riddle Me This by ILNP</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu5e33jfjgue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1jxp7ru</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Looking for regular polish with this vibe</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nmbzwr8ggue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1jxolbo</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>OPI - Coca-Cola Red</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hriu4gbfbgue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1jxo3gj</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Spring skittle</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60925coe7gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1jxnv31</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>You inspired me!!</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxnv31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1jxnedt</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Home-mixed polish peeling off in one sheet?</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j91i4z9w1gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1jxn3n0</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Desenio Pink posters</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxn3n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1jxmlul</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Cadillacquer - The Quiet Chaos</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxmlul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1jxmgzo</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Jurassic Park TONITE 4/12 @ 5PDT: https://discord.gg/redditlaqueristas</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8mxdlvmufue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1jxm4u9</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Inspired by Portia’s nails in White Lotus 🍵</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxm4u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1jxm1f8</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>I wanted to show you folks some of my favorite nails I've done over the past couple of months(:</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxm1f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1jxkfl3</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Help me color match this Matcha Nail Color</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mho9c9tnefue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1jxlqjm</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>I love one coat wonders!</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxlqjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1jxlawl</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>I finally found color!</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxlawl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1jxkr9g</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Did my coworkers hats to tease them, actually love the combo</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxkr9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1jxkisy</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>ILNP After Hours</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oegjmdsdffue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1jxk11r</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Am I missing any main colors?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxk11r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1jxjic4</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Comparison Request: ILNP Comet vs Mooncat Pangea</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jxjic4/comparison_request_ilnp_comet_vs_mooncat_pangea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1jxj5wa</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>My LynB order</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxj5wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1jximdz</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Lazy Daisies</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zitj5royzeue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1jxhvcx</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Orea by EdM</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vm00nhi9teue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1jxh999</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Going to a Vampire Museum so I tried to match my nails to the theme 🧛</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxh999</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1jxf3fe</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Reminds me of fountain pen ink/blueberries</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxf3fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1jxemaa</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Time for a palette cleanser</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxemaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1jx9aaz</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>OMG, Glitter Emergency! Which Iconic Sparkle Polish Screams YOUR Inner Unicorn Princess? 💅✨</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jx9aaz/omg_glitter_emergency_which_iconic_sparkle_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1jxa5zx</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Guess what arrive today? Sassy sauce order oh my God absolutely stunning colors wow. Even though they ended up being $30 each Canadian after the dollar exchange and the border crossing fees and taxes and shipping and blah blah blah but like I'm still pretty happy with the purchase</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxa5zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1jxdkpk</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Gels wrecked my nails 😩 Making the best of a bad situation!</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxdkpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1jxd7w9</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Resin dye / colourant in nail polish?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox11fkuledue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1jxcmjv</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Fire engine red?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jxcmjv/fire_engine_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1jxx2fe</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Easter Nails🐰</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxx2fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1jy13a0</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Disney Lorcana inspired nails</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6qfqqq66njue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1jy0krc</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>~illusion~</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mr55aixwgjue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1jxz2fc</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Frenchies for the warmer weather ☀️</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bipcq4wgziue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1jxxwba</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>What are the best press-on nails for a beginner?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jxxwba/what_are_the_best_presson_nails_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1jxxnjh</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Spring Set</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxxnjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1jxwj36</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>By Request Butterfly Nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swrspbky8iue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1jxw9k4</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Tried nail stamping for the first time. Sabrina Carpenter inspired</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxw9k4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1jxvven</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Blue China 💙</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxvven</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1jxund6</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Spring cuties 🐛🍄🐞🧡</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxund6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1jxtv5k</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>A Week Of Nails</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jxtv5k/a_week_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1jxtta5</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Beach nails! 🌊☀️🐚</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxtta5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1jxsimb</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Dark Vibes</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ocf1dmk7hue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1jxotbu</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Medieval gothic themed!!!</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxotbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1jxoryd</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Easter vibes for everyone</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxoryd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1jxnggp</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Froggy Inspo</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mf2h3yhc2gue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1jxn4nk</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Smoke and Mirrors</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxn4nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1jxlpp0</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Trend🤎✨</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9be9g8sofue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1jxhe0g</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Spring set!</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxhe0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1jxgcnz</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Toy Story Alien Nails!</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxgcnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1jxfjzj</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Looking to Master Nail Art – What Books Should I Read?</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jxfjzj/looking_to_master_nail_art_what_books_should_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1jxf48u</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>The nails I had for christmas ⭐️</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jxf48u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1jxf3de</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Aura nails firts try :)</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr7dbdob2eue1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>